<commit_message>
Reemplazo escaleta guion 1
Cambio escaleta con nuevas indicaciones: motores M101A en cada
consolidación y motor M101AP como banco de actividades.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion01/Escaleta_LE_09_01_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion01/Escaleta_LE_09_01_CO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="305">
   <si>
     <t>Asignatura</t>
   </si>
@@ -748,9 +748,6 @@
     <t>Recurso M5C-03</t>
   </si>
   <si>
-    <t>Recurso M101A-04</t>
-  </si>
-  <si>
     <t>Revisar las fichas DBA3</t>
   </si>
   <si>
@@ -869,13 +866,119 @@
   </si>
   <si>
     <t>Claves para la redacción de un comentario de texto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consolidación </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad para afianzar saberes sobre los autores y las obras de la literatura precolombina </t>
+  </si>
+  <si>
+    <t>Tres preguntas que tengan coherencia y se relacionen. Se puede indagar sobre los temas más empleados por los autores precolombinos y la forma como caracterizan personajes, su relación con la religión, las respuestas que buscan responder….</t>
+  </si>
+  <si>
+    <t>Recurso M</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Las oraciones simples y compuestas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refuerza tu aprendizaje: La literatura de la época precolombina </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proponer actividades de análisis de párrafos para identificar oraciones simples y compuestas. Luego, proponerles construir o escribir párrafos usando los dos tipos de oraciones. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad para afianzar la escritura de oraciones y párrafos </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Refuerza tu aprendizaje: las reglas ortográficas de los grafemas </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>g</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> y</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> j</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad para reconocer la escritura correcta de palabras con g y j </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proponer párrafos con las grafías g y j. Luego pedirles que expliquen qué regla se utilizó en cada caso. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad para desarrollar habilidades de lectura </t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje:  estrategias de lectura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proponer fragmentos cortos de comentario de texto y aplicar la estrategia de concluir, inferir algo a partir de ello. Proponer  preguntas puntuales que apunten a tales inferencias o conclusiones. </t>
+  </si>
+  <si>
+    <t>Recurso M101A-4</t>
+  </si>
+  <si>
+    <t>Recurso M101A-5</t>
+  </si>
+  <si>
+    <t>Recurso M101A-6</t>
+  </si>
+  <si>
+    <t>Recurso M101A-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El comentario de texto </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banco de actividades </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividades para repasar los contenidos del tema El comentario de texto </t>
+  </si>
+  <si>
+    <t>Debe incluirse 10 preguntas abiertas:3 sobre literatura; 2 sobre gramática, 2 de ortografía, 2 de Comprensión y 1 de producción.  Debe marcarse en el greco Gestor de actividades como actividad didáctica</t>
+  </si>
+  <si>
+    <t>Recurso M101AP</t>
+  </si>
+  <si>
+    <t>Recurso M101A-08</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -922,6 +1025,14 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1260,7 +1371,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1337,6 +1448,42 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1357,9 +1504,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -1651,10 +1795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U91"/>
+  <dimension ref="A1:U95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D32" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="R37" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="T42" sqref="T42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1681,94 +1825,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15" thickBot="1">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="H1" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="J1" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="55" t="s">
+      <c r="K1" s="75" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="53" t="s">
+      <c r="L1" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="52" t="s">
+      <c r="M1" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="52"/>
-      <c r="O1" s="50" t="s">
+      <c r="N1" s="72"/>
+      <c r="O1" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="50" t="s">
+      <c r="P1" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="50" t="s">
+      <c r="Q1" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="50" t="s">
+      <c r="R1" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="50" t="s">
+      <c r="S1" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="50" t="s">
+      <c r="T1" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="50" t="s">
+      <c r="U1" s="70" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="29.25" customHeight="1" thickBot="1">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="54"/>
+      <c r="A2" s="71"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="74"/>
       <c r="M2" s="17" t="s">
         <v>86</v>
       </c>
       <c r="N2" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="71"/>
+      <c r="Q2" s="71"/>
+      <c r="R2" s="71"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="71"/>
+      <c r="U2" s="71"/>
     </row>
     <row r="3" spans="1:21" ht="59" customHeight="1">
       <c r="A3" s="18" t="s">
@@ -1808,7 +1952,7 @@
       </c>
       <c r="N3" s="46"/>
       <c r="O3" s="46" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="P3" s="44" t="s">
         <v>19</v>
@@ -1867,7 +2011,7 @@
       </c>
       <c r="N4" s="46"/>
       <c r="O4" s="45" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="P4" s="44" t="s">
         <v>19</v>
@@ -2024,7 +2168,7 @@
       <c r="G7" s="35" t="s">
         <v>235</v>
       </c>
-      <c r="H7" s="36">
+      <c r="H7" s="33">
         <v>5</v>
       </c>
       <c r="I7" s="36" t="s">
@@ -2044,7 +2188,7 @@
       </c>
       <c r="N7" s="46"/>
       <c r="O7" s="45" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="P7" s="44" t="s">
         <v>19</v>
@@ -2103,7 +2247,7 @@
       </c>
       <c r="N8" s="46"/>
       <c r="O8" s="45" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="P8" s="44" t="s">
         <v>19</v>
@@ -2162,7 +2306,7 @@
         <v>35</v>
       </c>
       <c r="O9" s="45" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="P9" s="44" t="s">
         <v>19</v>
@@ -2196,8 +2340,8 @@
       <c r="D10" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="E10" s="57" t="s">
-        <v>277</v>
+      <c r="E10" s="50" t="s">
+        <v>276</v>
       </c>
       <c r="F10" s="29" t="s">
         <v>100</v>
@@ -2225,7 +2369,7 @@
         <v>44</v>
       </c>
       <c r="O10" s="45" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P10" s="44" t="s">
         <v>19</v>
@@ -2259,8 +2403,8 @@
       <c r="D11" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="E11" s="57" t="s">
-        <v>277</v>
+      <c r="E11" s="50" t="s">
+        <v>276</v>
       </c>
       <c r="F11" s="29" t="s">
         <v>100</v>
@@ -2268,7 +2412,7 @@
       <c r="G11" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="H11" s="36">
+      <c r="H11" s="33">
         <v>9</v>
       </c>
       <c r="I11" s="36" t="s">
@@ -2288,7 +2432,7 @@
       </c>
       <c r="N11" s="46"/>
       <c r="O11" s="45" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="P11" s="44" t="s">
         <v>19</v>
@@ -2322,8 +2466,8 @@
       <c r="D12" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="E12" s="57" t="s">
-        <v>277</v>
+      <c r="E12" s="50" t="s">
+        <v>276</v>
       </c>
       <c r="F12" s="29" t="s">
         <v>100</v>
@@ -2351,7 +2495,7 @@
       </c>
       <c r="N12" s="46"/>
       <c r="O12" s="45" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="P12" s="44" t="s">
         <v>19</v>
@@ -2385,8 +2529,8 @@
       <c r="D13" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="E13" s="57" t="s">
-        <v>278</v>
+      <c r="E13" s="50" t="s">
+        <v>277</v>
       </c>
       <c r="F13" s="29" t="s">
         <v>114</v>
@@ -2414,7 +2558,7 @@
       </c>
       <c r="N13" s="46"/>
       <c r="O13" s="45" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P13" s="44" t="s">
         <v>19</v>
@@ -2448,8 +2592,8 @@
       <c r="D14" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="E14" s="57" t="s">
-        <v>278</v>
+      <c r="E14" s="50" t="s">
+        <v>277</v>
       </c>
       <c r="F14" s="29" t="s">
         <v>118</v>
@@ -2477,7 +2621,7 @@
         <v>37</v>
       </c>
       <c r="O14" s="45" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="P14" s="44" t="s">
         <v>19</v>
@@ -2511,8 +2655,8 @@
       <c r="D15" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="E15" s="57" t="s">
-        <v>278</v>
+      <c r="E15" s="50" t="s">
+        <v>277</v>
       </c>
       <c r="F15" s="29" t="s">
         <v>118</v>
@@ -2520,7 +2664,7 @@
       <c r="G15" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="H15" s="36">
+      <c r="H15" s="33">
         <v>13</v>
       </c>
       <c r="I15" s="36" t="s">
@@ -2540,7 +2684,7 @@
       </c>
       <c r="N15" s="46"/>
       <c r="O15" s="45" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="P15" s="44" t="s">
         <v>20</v>
@@ -2561,68 +2705,68 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
-      <c r="A16" s="21" t="s">
+    <row r="16" spans="1:21" ht="56">
+      <c r="A16" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="E16" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="F16" s="29"/>
-      <c r="G16" s="35" t="s">
-        <v>129</v>
+      <c r="E16" s="55" t="s">
+        <v>281</v>
+      </c>
+      <c r="F16" s="56"/>
+      <c r="G16" s="39" t="s">
+        <v>286</v>
       </c>
       <c r="H16" s="36">
         <v>14</v>
       </c>
-      <c r="I16" s="36" t="s">
+      <c r="I16" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="J16" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="K16" s="42" t="s">
+      <c r="J16" s="58" t="s">
+        <v>282</v>
+      </c>
+      <c r="K16" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="L16" s="43" t="s">
+      <c r="L16" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="M16" s="46" t="s">
-        <v>74</v>
+      <c r="M16" s="61" t="s">
+        <v>62</v>
       </c>
       <c r="N16" s="46"/>
-      <c r="O16" s="45" t="s">
-        <v>253</v>
-      </c>
-      <c r="P16" s="44" t="s">
+      <c r="O16" s="62" t="s">
+        <v>283</v>
+      </c>
+      <c r="P16" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="Q16" s="1">
+      <c r="Q16" s="64">
         <v>6</v>
       </c>
-      <c r="R16" s="13" t="s">
+      <c r="R16" s="65" t="s">
         <v>107</v>
       </c>
-      <c r="S16" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="T16" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="U16" s="2" t="s">
+      <c r="S16" s="65" t="s">
+        <v>284</v>
+      </c>
+      <c r="T16" s="65" t="s">
+        <v>219</v>
+      </c>
+      <c r="U16" s="66" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="28">
+    <row r="17" spans="1:21">
       <c r="A17" s="21" t="s">
         <v>68</v>
       </c>
@@ -2632,51 +2776,55 @@
       <c r="C17" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="D17" s="47" t="s">
-        <v>128</v>
-      </c>
-      <c r="E17" s="28"/>
+      <c r="D17" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>125</v>
+      </c>
       <c r="F17" s="29"/>
       <c r="G17" s="35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H17" s="36">
         <v>15</v>
       </c>
       <c r="I17" s="36" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="J17" s="37" t="s">
-        <v>171</v>
+        <v>126</v>
       </c>
       <c r="K17" s="42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L17" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="M17" s="46"/>
+        <v>32</v>
+      </c>
+      <c r="M17" s="46" t="s">
+        <v>74</v>
+      </c>
       <c r="N17" s="46"/>
       <c r="O17" s="45" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="P17" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="Q17" s="1" t="s">
-        <v>131</v>
+      <c r="Q17" s="1">
+        <v>6</v>
       </c>
       <c r="R17" s="13" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="S17" s="13" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="T17" s="13" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="28">
@@ -2695,27 +2843,27 @@
       <c r="E18" s="28"/>
       <c r="F18" s="29"/>
       <c r="G18" s="35" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H18" s="36">
         <v>16</v>
       </c>
       <c r="I18" s="36" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="J18" s="37" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K18" s="42" t="s">
         <v>70</v>
       </c>
       <c r="L18" s="43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M18" s="46"/>
       <c r="N18" s="46"/>
       <c r="O18" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="P18" s="44" t="s">
         <v>19</v>
@@ -2730,7 +2878,7 @@
         <v>133</v>
       </c>
       <c r="T18" s="13" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="U18" s="2" t="s">
         <v>135</v>
@@ -2752,27 +2900,27 @@
       <c r="E19" s="28"/>
       <c r="F19" s="29"/>
       <c r="G19" s="35" t="s">
-        <v>139</v>
-      </c>
-      <c r="H19" s="36">
+        <v>136</v>
+      </c>
+      <c r="H19" s="33">
         <v>17</v>
       </c>
       <c r="I19" s="36" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="J19" s="37" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K19" s="42" t="s">
         <v>70</v>
       </c>
       <c r="L19" s="43" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M19" s="46"/>
       <c r="N19" s="46"/>
       <c r="O19" s="45" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="P19" s="44" t="s">
         <v>19</v>
@@ -2787,7 +2935,7 @@
         <v>133</v>
       </c>
       <c r="T19" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U19" s="2" t="s">
         <v>135</v>
@@ -2809,27 +2957,27 @@
       <c r="E20" s="28"/>
       <c r="F20" s="29"/>
       <c r="G20" s="35" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H20" s="36">
         <v>18</v>
       </c>
       <c r="I20" s="36" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="J20" s="37" t="s">
-        <v>144</v>
+        <v>173</v>
       </c>
       <c r="K20" s="42" t="s">
         <v>70</v>
       </c>
       <c r="L20" s="43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M20" s="46"/>
       <c r="N20" s="46"/>
       <c r="O20" s="45" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="P20" s="44" t="s">
         <v>19</v>
@@ -2841,13 +2989,13 @@
         <v>132</v>
       </c>
       <c r="S20" s="13" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="T20" s="13" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="U20" s="2" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="28">
@@ -2866,7 +3014,7 @@
       <c r="E21" s="28"/>
       <c r="F21" s="29"/>
       <c r="G21" s="35" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="H21" s="36">
         <v>19</v>
@@ -2875,7 +3023,7 @@
         <v>105</v>
       </c>
       <c r="J21" s="37" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="K21" s="42" t="s">
         <v>70</v>
@@ -2886,7 +3034,7 @@
       <c r="M21" s="46"/>
       <c r="N21" s="46"/>
       <c r="O21" s="45" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="P21" s="44" t="s">
         <v>19</v>
@@ -2901,7 +3049,7 @@
         <v>141</v>
       </c>
       <c r="T21" s="13" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="U21" s="2" t="s">
         <v>143</v>
@@ -2923,27 +3071,27 @@
       <c r="E22" s="28"/>
       <c r="F22" s="29"/>
       <c r="G22" s="35" t="s">
-        <v>176</v>
+        <v>145</v>
       </c>
       <c r="H22" s="36">
         <v>20</v>
       </c>
       <c r="I22" s="36" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="J22" s="37" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K22" s="42" t="s">
         <v>70</v>
       </c>
       <c r="L22" s="43" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M22" s="46"/>
       <c r="N22" s="46"/>
       <c r="O22" s="45" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="P22" s="44" t="s">
         <v>19</v>
@@ -2958,13 +3106,13 @@
         <v>141</v>
       </c>
       <c r="T22" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="U22" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="70">
+    <row r="23" spans="1:21" ht="28">
       <c r="A23" s="21" t="s">
         <v>68</v>
       </c>
@@ -2977,112 +3125,112 @@
       <c r="D23" s="47" t="s">
         <v>128</v>
       </c>
-      <c r="E23" s="28" t="s">
-        <v>125</v>
-      </c>
+      <c r="E23" s="28"/>
       <c r="F23" s="29"/>
       <c r="G23" s="35" t="s">
-        <v>148</v>
-      </c>
-      <c r="H23" s="36">
+        <v>176</v>
+      </c>
+      <c r="H23" s="33">
         <v>21</v>
       </c>
       <c r="I23" s="36" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="J23" s="37" t="s">
-        <v>149</v>
+        <v>175</v>
       </c>
       <c r="K23" s="42" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L23" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M23" s="46" t="s">
-        <v>47</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="M23" s="46"/>
       <c r="N23" s="46"/>
       <c r="O23" s="45" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="P23" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="1">
-        <v>6</v>
+      <c r="Q23" s="1" t="s">
+        <v>131</v>
       </c>
       <c r="R23" s="13" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
       <c r="S23" s="13" t="s">
-        <v>108</v>
+        <v>141</v>
       </c>
       <c r="T23" s="13" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="U23" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" ht="28">
-      <c r="A24" s="21" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="42">
+      <c r="A24" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="24" t="s">
-        <v>151</v>
-      </c>
-      <c r="E24" s="28"/>
+      <c r="D24" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="68" t="s">
+        <v>281</v>
+      </c>
       <c r="F24" s="29"/>
-      <c r="G24" s="35" t="s">
-        <v>152</v>
+      <c r="G24" s="39" t="s">
+        <v>285</v>
       </c>
       <c r="H24" s="36">
         <v>22</v>
       </c>
-      <c r="I24" s="36" t="s">
-        <v>94</v>
-      </c>
-      <c r="J24" s="37" t="s">
-        <v>153</v>
-      </c>
-      <c r="K24" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="L24" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="M24" s="46"/>
+      <c r="I24" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="J24" s="58" t="s">
+        <v>288</v>
+      </c>
+      <c r="K24" s="59" t="s">
+        <v>69</v>
+      </c>
+      <c r="L24" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="M24" s="61" t="s">
+        <v>62</v>
+      </c>
       <c r="N24" s="46"/>
-      <c r="O24" s="45" t="s">
-        <v>180</v>
-      </c>
-      <c r="P24" s="44" t="s">
+      <c r="O24" s="62" t="s">
+        <v>287</v>
+      </c>
+      <c r="P24" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="Q24" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="R24" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="S24" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="T24" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="U24" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21">
+      <c r="Q24" s="64">
+        <v>6</v>
+      </c>
+      <c r="R24" s="65" t="s">
+        <v>107</v>
+      </c>
+      <c r="S24" s="65" t="s">
+        <v>284</v>
+      </c>
+      <c r="T24" s="65" t="s">
+        <v>295</v>
+      </c>
+      <c r="U24" s="66" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="70">
       <c r="A25" s="21" t="s">
         <v>68</v>
       </c>
@@ -3092,15 +3240,15 @@
       <c r="C25" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="D25" s="24" t="s">
-        <v>151</v>
+      <c r="D25" s="47" t="s">
+        <v>128</v>
       </c>
       <c r="E25" s="28" t="s">
-        <v>158</v>
+        <v>125</v>
       </c>
       <c r="F25" s="29"/>
       <c r="G25" s="35" t="s">
-        <v>177</v>
+        <v>148</v>
       </c>
       <c r="H25" s="36">
         <v>23</v>
@@ -3109,39 +3257,41 @@
         <v>105</v>
       </c>
       <c r="J25" s="37" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="K25" s="42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L25" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="M25" s="46"/>
+      <c r="M25" s="46" t="s">
+        <v>47</v>
+      </c>
       <c r="N25" s="46"/>
       <c r="O25" s="45" t="s">
-        <v>178</v>
+        <v>258</v>
       </c>
       <c r="P25" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="Q25" s="1" t="s">
-        <v>131</v>
+      <c r="Q25" s="1">
+        <v>6</v>
       </c>
       <c r="R25" s="13" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="S25" s="13" t="s">
-        <v>154</v>
+        <v>108</v>
       </c>
       <c r="T25" s="13" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="U25" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" ht="84">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="28">
       <c r="A26" s="21" t="s">
         <v>68</v>
       </c>
@@ -3154,52 +3304,48 @@
       <c r="D26" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="E26" s="28" t="s">
-        <v>158</v>
-      </c>
+      <c r="E26" s="28"/>
       <c r="F26" s="29"/>
       <c r="G26" s="35" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="H26" s="36">
         <v>24</v>
       </c>
       <c r="I26" s="36" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="J26" s="37" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="K26" s="42" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L26" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M26" s="46" t="s">
-        <v>83</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="M26" s="46"/>
       <c r="N26" s="46"/>
       <c r="O26" s="45" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
       <c r="P26" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="1">
-        <v>6</v>
+      <c r="Q26" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="R26" s="13" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
       <c r="S26" s="13" t="s">
-        <v>108</v>
+        <v>182</v>
       </c>
       <c r="T26" s="13" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="U26" s="2" t="s">
-        <v>110</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="1:21">
@@ -3216,20 +3362,20 @@
         <v>151</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="F27" s="29"/>
       <c r="G27" s="35" t="s">
-        <v>163</v>
-      </c>
-      <c r="H27" s="36">
+        <v>177</v>
+      </c>
+      <c r="H27" s="33">
         <v>25</v>
       </c>
       <c r="I27" s="36" t="s">
         <v>105</v>
       </c>
       <c r="J27" s="37" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
       <c r="K27" s="42" t="s">
         <v>70</v>
@@ -3240,7 +3386,7 @@
       <c r="M27" s="46"/>
       <c r="N27" s="46"/>
       <c r="O27" s="45" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="P27" s="44" t="s">
         <v>19</v>
@@ -3255,13 +3401,13 @@
         <v>154</v>
       </c>
       <c r="T27" s="13" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="U27" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:21" ht="84">
       <c r="A28" s="21" t="s">
         <v>68</v>
       </c>
@@ -3275,11 +3421,11 @@
         <v>151</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="F28" s="29"/>
       <c r="G28" s="35" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="H28" s="36">
         <v>26</v>
@@ -3288,36 +3434,38 @@
         <v>105</v>
       </c>
       <c r="J28" s="37" t="s">
-        <v>260</v>
+        <v>160</v>
       </c>
       <c r="K28" s="42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L28" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="M28" s="46"/>
+      <c r="M28" s="46" t="s">
+        <v>83</v>
+      </c>
       <c r="N28" s="46"/>
       <c r="O28" s="45" t="s">
-        <v>137</v>
+        <v>161</v>
       </c>
       <c r="P28" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>131</v>
+        <v>19</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>6</v>
       </c>
       <c r="R28" s="13" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="S28" s="13" t="s">
-        <v>154</v>
+        <v>108</v>
       </c>
       <c r="T28" s="13" t="s">
-        <v>167</v>
+        <v>192</v>
       </c>
       <c r="U28" s="2" t="s">
-        <v>156</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:21">
@@ -3331,118 +3479,116 @@
         <v>91</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>279</v>
+        <v>151</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>168</v>
+        <v>125</v>
       </c>
       <c r="F29" s="29"/>
       <c r="G29" s="35" t="s">
-        <v>91</v>
+        <v>163</v>
       </c>
       <c r="H29" s="36">
         <v>27</v>
       </c>
       <c r="I29" s="36" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="J29" s="37" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="K29" s="42" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L29" s="43" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M29" s="46"/>
-      <c r="N29" s="46" t="s">
-        <v>37</v>
-      </c>
+      <c r="N29" s="46"/>
       <c r="O29" s="45" t="s">
-        <v>261</v>
+        <v>164</v>
       </c>
       <c r="P29" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="Q29" s="1">
-        <v>6</v>
+      <c r="Q29" s="1" t="s">
+        <v>131</v>
       </c>
       <c r="R29" s="13" t="s">
-        <v>96</v>
+        <v>132</v>
       </c>
       <c r="S29" s="13" t="s">
-        <v>97</v>
+        <v>154</v>
       </c>
       <c r="T29" s="13" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="U29" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" ht="70">
-      <c r="A30" s="21" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="28">
+      <c r="A30" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="C30" s="23" t="s">
+      <c r="C30" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="D30" s="24" t="s">
-        <v>279</v>
-      </c>
-      <c r="E30" s="28" t="s">
-        <v>185</v>
+      <c r="D30" s="54" t="s">
+        <v>151</v>
+      </c>
+      <c r="E30" s="68" t="s">
+        <v>125</v>
       </c>
       <c r="F30" s="29"/>
       <c r="G30" s="39" t="s">
-        <v>186</v>
+        <v>289</v>
       </c>
       <c r="H30" s="36">
         <v>28</v>
       </c>
-      <c r="I30" s="36" t="s">
+      <c r="I30" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="J30" s="37" t="s">
-        <v>187</v>
-      </c>
-      <c r="K30" s="42" t="s">
+      <c r="J30" s="58" t="s">
+        <v>290</v>
+      </c>
+      <c r="K30" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="L30" s="43" t="s">
+      <c r="L30" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="M30" s="46" t="s">
-        <v>64</v>
+      <c r="M30" s="61" t="s">
+        <v>62</v>
       </c>
       <c r="N30" s="46"/>
-      <c r="O30" s="45" t="s">
-        <v>262</v>
-      </c>
-      <c r="P30" s="44" t="s">
+      <c r="O30" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="P30" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="Q30" s="1">
+      <c r="Q30" s="64">
         <v>6</v>
       </c>
-      <c r="R30" s="13" t="s">
+      <c r="R30" s="65" t="s">
         <v>107</v>
       </c>
-      <c r="S30" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="T30" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="U30" s="2" t="s">
+      <c r="S30" s="65" t="s">
+        <v>284</v>
+      </c>
+      <c r="T30" s="65" t="s">
+        <v>296</v>
+      </c>
+      <c r="U30" s="66" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="42">
+    <row r="31" spans="1:21">
       <c r="A31" s="21" t="s">
         <v>68</v>
       </c>
@@ -3453,57 +3599,55 @@
         <v>91</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>279</v>
+        <v>151</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>189</v>
+        <v>125</v>
       </c>
       <c r="F31" s="29"/>
       <c r="G31" s="35" t="s">
-        <v>190</v>
-      </c>
-      <c r="H31" s="36">
+        <v>166</v>
+      </c>
+      <c r="H31" s="33">
         <v>29</v>
       </c>
       <c r="I31" s="36" t="s">
         <v>105</v>
       </c>
       <c r="J31" s="37" t="s">
-        <v>191</v>
+        <v>259</v>
       </c>
       <c r="K31" s="42" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L31" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="M31" s="46" t="s">
-        <v>83</v>
-      </c>
+      <c r="M31" s="46"/>
       <c r="N31" s="46"/>
       <c r="O31" s="45" t="s">
-        <v>263</v>
+        <v>137</v>
       </c>
       <c r="P31" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="Q31" s="1">
-        <v>6</v>
+      <c r="Q31" s="1" t="s">
+        <v>131</v>
       </c>
       <c r="R31" s="13" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
       <c r="S31" s="13" t="s">
-        <v>108</v>
+        <v>154</v>
       </c>
       <c r="T31" s="13" t="s">
-        <v>240</v>
+        <v>167</v>
       </c>
       <c r="U31" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" ht="28">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
       <c r="A32" s="21" t="s">
         <v>68</v>
       </c>
@@ -3514,36 +3658,36 @@
         <v>91</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E32" s="28" t="s">
-        <v>125</v>
+        <v>168</v>
       </c>
       <c r="F32" s="29"/>
       <c r="G32" s="35" t="s">
-        <v>193</v>
+        <v>91</v>
       </c>
       <c r="H32" s="36">
         <v>30</v>
       </c>
       <c r="I32" s="36" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="J32" s="37" t="s">
-        <v>194</v>
+        <v>169</v>
       </c>
       <c r="K32" s="42" t="s">
         <v>69</v>
       </c>
       <c r="L32" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M32" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="N32" s="46"/>
+        <v>31</v>
+      </c>
+      <c r="M32" s="46"/>
+      <c r="N32" s="46" t="s">
+        <v>37</v>
+      </c>
       <c r="O32" s="45" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="P32" s="44" t="s">
         <v>19</v>
@@ -3552,19 +3696,19 @@
         <v>6</v>
       </c>
       <c r="R32" s="13" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="S32" s="13" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="T32" s="13" t="s">
-        <v>195</v>
+        <v>170</v>
       </c>
       <c r="U32" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" ht="70">
       <c r="A33" s="21" t="s">
         <v>68</v>
       </c>
@@ -3575,55 +3719,57 @@
         <v>91</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="F33" s="29"/>
-      <c r="G33" s="35" t="s">
-        <v>197</v>
+      <c r="G33" s="69" t="s">
+        <v>186</v>
       </c>
       <c r="H33" s="36">
+        <v>31</v>
+      </c>
+      <c r="I33" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="J33" s="37" t="s">
+        <v>187</v>
+      </c>
+      <c r="K33" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="L33" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="I33" s="36" t="s">
-        <v>94</v>
-      </c>
-      <c r="J33" s="37" t="s">
-        <v>207</v>
-      </c>
-      <c r="K33" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="L33" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="M33" s="46"/>
+      <c r="M33" s="46" t="s">
+        <v>64</v>
+      </c>
       <c r="N33" s="46"/>
       <c r="O33" s="45" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="P33" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="Q33" s="1" t="s">
-        <v>208</v>
+      <c r="Q33" s="1">
+        <v>6</v>
       </c>
       <c r="R33" s="13" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="S33" s="13" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="T33" s="13" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="U33" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" ht="28">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" ht="42">
       <c r="A34" s="21" t="s">
         <v>68</v>
       </c>
@@ -3634,118 +3780,118 @@
         <v>91</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E34" s="28" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="F34" s="29"/>
       <c r="G34" s="35" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
       <c r="H34" s="36">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I34" s="36" t="s">
         <v>105</v>
       </c>
       <c r="J34" s="37" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
       <c r="K34" s="42" t="s">
         <v>69</v>
       </c>
       <c r="L34" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="M34" s="46"/>
-      <c r="N34" s="46" t="s">
-        <v>46</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="M34" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="N34" s="46"/>
       <c r="O34" s="45" t="s">
-        <v>214</v>
+        <v>262</v>
       </c>
       <c r="P34" s="44" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q34" s="1">
         <v>6</v>
       </c>
       <c r="R34" s="13" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="S34" s="13" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="T34" s="13" t="s">
-        <v>213</v>
+        <v>240</v>
       </c>
       <c r="U34" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" ht="56">
-      <c r="A35" s="21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" ht="42">
+      <c r="A35" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="23" t="s">
+      <c r="C35" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="D35" s="24" t="s">
-        <v>280</v>
-      </c>
-      <c r="E35" s="28" t="s">
-        <v>125</v>
+      <c r="D35" s="54" t="s">
+        <v>278</v>
+      </c>
+      <c r="E35" s="68" t="s">
+        <v>281</v>
       </c>
       <c r="F35" s="29"/>
-      <c r="G35" s="35" t="s">
-        <v>198</v>
-      </c>
-      <c r="H35" s="36">
+      <c r="G35" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="H35" s="33">
         <v>33</v>
       </c>
-      <c r="I35" s="36" t="s">
+      <c r="I35" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="J35" s="37" t="s">
-        <v>199</v>
-      </c>
-      <c r="K35" s="42" t="s">
+      <c r="J35" s="58" t="s">
+        <v>292</v>
+      </c>
+      <c r="K35" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="L35" s="43" t="s">
+      <c r="L35" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="M35" s="46" t="s">
+      <c r="M35" s="61" t="s">
         <v>62</v>
       </c>
       <c r="N35" s="46"/>
-      <c r="O35" s="45" t="s">
-        <v>215</v>
-      </c>
-      <c r="P35" s="44" t="s">
+      <c r="O35" s="62" t="s">
+        <v>294</v>
+      </c>
+      <c r="P35" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="Q35" s="1">
+      <c r="Q35" s="64">
         <v>6</v>
       </c>
-      <c r="R35" s="13" t="s">
+      <c r="R35" s="65" t="s">
         <v>107</v>
       </c>
-      <c r="S35" s="13" t="s">
+      <c r="S35" s="65" t="s">
         <v>108</v>
       </c>
-      <c r="T35" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="U35" s="2" t="s">
+      <c r="T35" s="65" t="s">
+        <v>297</v>
+      </c>
+      <c r="U35" s="66" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="36" spans="1:21">
+    <row r="36" spans="1:21" ht="28">
       <c r="A36" s="21" t="s">
         <v>68</v>
       </c>
@@ -3756,12 +3902,14 @@
         <v>91</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>201</v>
-      </c>
-      <c r="E36" s="28"/>
+        <v>278</v>
+      </c>
+      <c r="E36" s="28" t="s">
+        <v>125</v>
+      </c>
       <c r="F36" s="29"/>
       <c r="G36" s="35" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="H36" s="36">
         <v>34</v>
@@ -3769,8 +3917,8 @@
       <c r="I36" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="J36" s="34" t="s">
-        <v>203</v>
+      <c r="J36" s="37" t="s">
+        <v>194</v>
       </c>
       <c r="K36" s="42" t="s">
         <v>69</v>
@@ -3779,11 +3927,11 @@
         <v>32</v>
       </c>
       <c r="M36" s="46" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="N36" s="46"/>
       <c r="O36" s="45" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="P36" s="44" t="s">
         <v>19</v>
@@ -3798,7 +3946,7 @@
         <v>108</v>
       </c>
       <c r="T36" s="13" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="U36" s="2" t="s">
         <v>110</v>
@@ -3815,53 +3963,55 @@
         <v>91</v>
       </c>
       <c r="D37" s="24" t="s">
-        <v>201</v>
-      </c>
-      <c r="E37" s="28"/>
+        <v>279</v>
+      </c>
+      <c r="E37" s="28" t="s">
+        <v>196</v>
+      </c>
       <c r="F37" s="29"/>
       <c r="G37" s="35" t="s">
-        <v>139</v>
+        <v>197</v>
       </c>
       <c r="H37" s="36">
         <v>35</v>
       </c>
       <c r="I37" s="36" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="J37" s="37" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="K37" s="42" t="s">
         <v>70</v>
       </c>
       <c r="L37" s="43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M37" s="46"/>
       <c r="N37" s="46"/>
       <c r="O37" s="45" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="P37" s="44" t="s">
         <v>19</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>131</v>
+        <v>208</v>
       </c>
       <c r="R37" s="13" t="s">
         <v>132</v>
       </c>
       <c r="S37" s="13" t="s">
-        <v>141</v>
+        <v>91</v>
       </c>
       <c r="T37" s="13" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="U37" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" ht="84">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" ht="28">
       <c r="A38" s="21" t="s">
         <v>68</v>
       </c>
@@ -3872,12 +4022,14 @@
         <v>91</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>201</v>
-      </c>
-      <c r="E38" s="28"/>
+        <v>279</v>
+      </c>
+      <c r="E38" s="28" t="s">
+        <v>196</v>
+      </c>
       <c r="F38" s="29"/>
       <c r="G38" s="35" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="H38" s="36">
         <v>36</v>
@@ -3886,20 +4038,20 @@
         <v>105</v>
       </c>
       <c r="J38" s="37" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K38" s="42" t="s">
         <v>69</v>
       </c>
       <c r="L38" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M38" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="N38" s="46"/>
+        <v>31</v>
+      </c>
+      <c r="M38" s="46"/>
+      <c r="N38" s="46" t="s">
+        <v>46</v>
+      </c>
       <c r="O38" s="45" t="s">
-        <v>268</v>
+        <v>214</v>
       </c>
       <c r="P38" s="44" t="s">
         <v>19</v>
@@ -3908,19 +4060,19 @@
         <v>6</v>
       </c>
       <c r="R38" s="13" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="S38" s="13" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="T38" s="13" t="s">
-        <v>241</v>
+        <v>213</v>
       </c>
       <c r="U38" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" ht="42">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" ht="56">
       <c r="A39" s="21" t="s">
         <v>68</v>
       </c>
@@ -3931,21 +4083,23 @@
         <v>91</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>201</v>
-      </c>
-      <c r="E39" s="28"/>
+        <v>279</v>
+      </c>
+      <c r="E39" s="28" t="s">
+        <v>125</v>
+      </c>
       <c r="F39" s="29"/>
       <c r="G39" s="35" t="s">
-        <v>281</v>
-      </c>
-      <c r="H39" s="36">
+        <v>198</v>
+      </c>
+      <c r="H39" s="33">
         <v>37</v>
       </c>
       <c r="I39" s="36" t="s">
         <v>105</v>
       </c>
       <c r="J39" s="37" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
       <c r="K39" s="42" t="s">
         <v>69</v>
@@ -3954,11 +4108,11 @@
         <v>32</v>
       </c>
       <c r="M39" s="46" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="N39" s="46"/>
       <c r="O39" s="45" t="s">
-        <v>269</v>
+        <v>215</v>
       </c>
       <c r="P39" s="44" t="s">
         <v>19</v>
@@ -3972,8 +4126,8 @@
       <c r="S39" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="T39" s="13" t="s">
-        <v>216</v>
+      <c r="T39" s="65" t="s">
+        <v>298</v>
       </c>
       <c r="U39" s="2" t="s">
         <v>110</v>
@@ -3990,12 +4144,12 @@
         <v>91</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>270</v>
+        <v>201</v>
       </c>
       <c r="E40" s="28"/>
       <c r="F40" s="29"/>
       <c r="G40" s="35" t="s">
-        <v>271</v>
+        <v>202</v>
       </c>
       <c r="H40" s="36">
         <v>38</v>
@@ -4003,26 +4157,40 @@
       <c r="I40" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="J40" s="37" t="s">
-        <v>272</v>
+      <c r="J40" s="34" t="s">
+        <v>203</v>
       </c>
       <c r="K40" s="42" t="s">
         <v>69</v>
       </c>
       <c r="L40" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="M40" s="46"/>
+        <v>32</v>
+      </c>
+      <c r="M40" s="46" t="s">
+        <v>53</v>
+      </c>
       <c r="N40" s="46"/>
-      <c r="O40" s="45"/>
+      <c r="O40" s="45" t="s">
+        <v>265</v>
+      </c>
       <c r="P40" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="Q40" s="1"/>
-      <c r="R40" s="13"/>
-      <c r="S40" s="13"/>
-      <c r="T40" s="13"/>
-      <c r="U40" s="2"/>
+      <c r="Q40" s="1">
+        <v>6</v>
+      </c>
+      <c r="R40" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="S40" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="T40" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="U40" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="41" spans="1:21">
       <c r="A41" s="21" t="s">
@@ -4035,12 +4203,12 @@
         <v>91</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>270</v>
+        <v>201</v>
       </c>
       <c r="E41" s="28"/>
       <c r="F41" s="29"/>
       <c r="G41" s="35" t="s">
-        <v>273</v>
+        <v>139</v>
       </c>
       <c r="H41" s="36">
         <v>39</v>
@@ -4049,103 +4217,195 @@
         <v>105</v>
       </c>
       <c r="J41" s="37" t="s">
-        <v>274</v>
+        <v>205</v>
       </c>
       <c r="K41" s="42" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L41" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="M41" s="46" t="s">
-        <v>23</v>
-      </c>
+      <c r="M41" s="46"/>
       <c r="N41" s="46"/>
       <c r="O41" s="45" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="P41" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="Q41" s="1">
-        <v>6</v>
+      <c r="Q41" s="1" t="s">
+        <v>131</v>
       </c>
       <c r="R41" s="13" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
       <c r="S41" s="13" t="s">
-        <v>108</v>
+        <v>141</v>
       </c>
       <c r="T41" s="13" t="s">
-        <v>276</v>
+        <v>206</v>
       </c>
       <c r="U41" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" s="5" customFormat="1">
-      <c r="A42" s="21"/>
-      <c r="B42" s="19"/>
-      <c r="C42" s="23"/>
-      <c r="D42" s="24"/>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" ht="84">
+      <c r="A42" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="D42" s="24" t="s">
+        <v>201</v>
+      </c>
       <c r="E42" s="28"/>
       <c r="F42" s="29"/>
-      <c r="G42" s="35"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="37"/>
-      <c r="K42" s="42"/>
-      <c r="L42" s="43"/>
-      <c r="M42" s="46"/>
+      <c r="G42" s="35" t="s">
+        <v>217</v>
+      </c>
+      <c r="H42" s="36">
+        <v>40</v>
+      </c>
+      <c r="I42" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="J42" s="37" t="s">
+        <v>218</v>
+      </c>
+      <c r="K42" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="L42" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="M42" s="46" t="s">
+        <v>62</v>
+      </c>
       <c r="N42" s="46"/>
-      <c r="O42" s="45"/>
-      <c r="P42" s="44"/>
-      <c r="Q42" s="1"/>
-      <c r="R42" s="13"/>
-      <c r="S42" s="13"/>
-      <c r="T42" s="13"/>
-      <c r="U42" s="2"/>
-    </row>
-    <row r="43" spans="1:21">
-      <c r="A43" s="21"/>
-      <c r="B43" s="22"/>
-      <c r="C43" s="23"/>
-      <c r="D43" s="24"/>
+      <c r="O42" s="45" t="s">
+        <v>267</v>
+      </c>
+      <c r="P42" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q42" s="1">
+        <v>6</v>
+      </c>
+      <c r="R42" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="S42" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="T42" s="65" t="s">
+        <v>304</v>
+      </c>
+      <c r="U42" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" ht="42">
+      <c r="A43" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" s="24" t="s">
+        <v>201</v>
+      </c>
       <c r="E43" s="28"/>
       <c r="F43" s="29"/>
-      <c r="G43" s="35"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="37"/>
-      <c r="K43" s="42"/>
-      <c r="L43" s="43"/>
-      <c r="M43" s="46"/>
+      <c r="G43" s="35" t="s">
+        <v>280</v>
+      </c>
+      <c r="H43" s="33">
+        <v>41</v>
+      </c>
+      <c r="I43" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="J43" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="K43" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="L43" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="M43" s="46" t="s">
+        <v>23</v>
+      </c>
       <c r="N43" s="46"/>
-      <c r="O43" s="45"/>
-      <c r="P43" s="44"/>
-      <c r="Q43" s="1"/>
-      <c r="R43" s="13"/>
-      <c r="S43" s="13"/>
-      <c r="T43" s="13"/>
-      <c r="U43" s="2"/>
+      <c r="O43" s="45" t="s">
+        <v>268</v>
+      </c>
+      <c r="P43" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q43" s="1">
+        <v>6</v>
+      </c>
+      <c r="R43" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="S43" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="T43" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="U43" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="44" spans="1:21">
-      <c r="A44" s="21"/>
-      <c r="B44" s="22"/>
-      <c r="C44" s="23"/>
-      <c r="D44" s="24"/>
+      <c r="A44" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44" s="24" t="s">
+        <v>269</v>
+      </c>
       <c r="E44" s="28"/>
       <c r="F44" s="29"/>
-      <c r="G44" s="35"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="37"/>
-      <c r="K44" s="42"/>
-      <c r="L44" s="43"/>
+      <c r="G44" s="35" t="s">
+        <v>270</v>
+      </c>
+      <c r="H44" s="36">
+        <v>42</v>
+      </c>
+      <c r="I44" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="J44" s="37" t="s">
+        <v>271</v>
+      </c>
+      <c r="K44" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="L44" s="43" t="s">
+        <v>33</v>
+      </c>
       <c r="M44" s="46"/>
       <c r="N44" s="46"/>
       <c r="O44" s="45"/>
-      <c r="P44" s="44"/>
+      <c r="P44" s="44" t="s">
+        <v>19</v>
+      </c>
       <c r="Q44" s="1"/>
       <c r="R44" s="13"/>
       <c r="S44" s="13"/>
@@ -4153,58 +4413,128 @@
       <c r="U44" s="2"/>
     </row>
     <row r="45" spans="1:21">
-      <c r="A45" s="21"/>
-      <c r="B45" s="22"/>
-      <c r="C45" s="23"/>
-      <c r="D45" s="24"/>
+      <c r="A45" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="D45" s="24" t="s">
+        <v>269</v>
+      </c>
       <c r="E45" s="28"/>
       <c r="F45" s="29"/>
-      <c r="G45" s="35"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="37"/>
-      <c r="K45" s="42"/>
-      <c r="L45" s="43"/>
-      <c r="M45" s="46"/>
+      <c r="G45" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="H45" s="36">
+        <v>43</v>
+      </c>
+      <c r="I45" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="J45" s="37" t="s">
+        <v>273</v>
+      </c>
+      <c r="K45" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="L45" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="M45" s="46" t="s">
+        <v>23</v>
+      </c>
       <c r="N45" s="46"/>
-      <c r="O45" s="45"/>
-      <c r="P45" s="44"/>
-      <c r="Q45" s="1"/>
-      <c r="R45" s="13"/>
-      <c r="S45" s="13"/>
-      <c r="T45" s="13"/>
-      <c r="U45" s="2"/>
-    </row>
-    <row r="46" spans="1:21">
-      <c r="A46" s="21"/>
-      <c r="B46" s="22"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="30"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="35"/>
-      <c r="H46" s="36"/>
-      <c r="I46" s="36"/>
-      <c r="J46" s="37"/>
-      <c r="K46" s="42"/>
-      <c r="L46" s="43"/>
-      <c r="M46" s="46"/>
-      <c r="N46" s="46"/>
-      <c r="O46" s="45"/>
-      <c r="P46" s="44"/>
-      <c r="Q46" s="1"/>
-      <c r="R46" s="13"/>
-      <c r="S46" s="13"/>
-      <c r="T46" s="13"/>
-      <c r="U46" s="2"/>
+      <c r="O45" s="45" t="s">
+        <v>274</v>
+      </c>
+      <c r="P45" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q45" s="1">
+        <v>6</v>
+      </c>
+      <c r="R45" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="S45" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="T45" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="U45" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" s="5" customFormat="1" ht="42">
+      <c r="A46" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="53" t="s">
+        <v>299</v>
+      </c>
+      <c r="D46" s="54" t="s">
+        <v>300</v>
+      </c>
+      <c r="E46" s="68"/>
+      <c r="F46" s="56"/>
+      <c r="G46" s="39"/>
+      <c r="H46" s="36">
+        <v>44</v>
+      </c>
+      <c r="I46" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="J46" s="58" t="s">
+        <v>301</v>
+      </c>
+      <c r="K46" s="59" t="s">
+        <v>69</v>
+      </c>
+      <c r="L46" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="M46" s="61" t="s">
+        <v>63</v>
+      </c>
+      <c r="N46" s="61"/>
+      <c r="O46" s="62" t="s">
+        <v>302</v>
+      </c>
+      <c r="P46" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q46" s="64">
+        <v>6</v>
+      </c>
+      <c r="R46" s="65" t="s">
+        <v>107</v>
+      </c>
+      <c r="S46" s="65" t="s">
+        <v>284</v>
+      </c>
+      <c r="T46" s="65" t="s">
+        <v>303</v>
+      </c>
+      <c r="U46" s="66" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="47" spans="1:21">
       <c r="A47" s="21"/>
       <c r="B47" s="22"/>
       <c r="C47" s="23"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="31"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="29"/>
       <c r="G47" s="35"/>
       <c r="H47" s="36"/>
       <c r="I47" s="36"/>
@@ -4225,9 +4555,9 @@
       <c r="A48" s="21"/>
       <c r="B48" s="22"/>
       <c r="C48" s="23"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="30"/>
-      <c r="F48" s="31"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="28"/>
+      <c r="F48" s="29"/>
       <c r="G48" s="35"/>
       <c r="H48" s="36"/>
       <c r="I48" s="36"/>
@@ -4248,9 +4578,9 @@
       <c r="A49" s="21"/>
       <c r="B49" s="22"/>
       <c r="C49" s="23"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="31"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="29"/>
       <c r="G49" s="35"/>
       <c r="H49" s="36"/>
       <c r="I49" s="36"/>
@@ -5232,6 +5562,98 @@
       <c r="S91" s="13"/>
       <c r="T91" s="13"/>
       <c r="U91" s="2"/>
+    </row>
+    <row r="92" spans="1:21">
+      <c r="A92" s="21"/>
+      <c r="B92" s="22"/>
+      <c r="C92" s="23"/>
+      <c r="D92" s="25"/>
+      <c r="E92" s="30"/>
+      <c r="F92" s="31"/>
+      <c r="G92" s="35"/>
+      <c r="H92" s="36"/>
+      <c r="I92" s="36"/>
+      <c r="J92" s="37"/>
+      <c r="K92" s="42"/>
+      <c r="L92" s="43"/>
+      <c r="M92" s="46"/>
+      <c r="N92" s="46"/>
+      <c r="O92" s="45"/>
+      <c r="P92" s="44"/>
+      <c r="Q92" s="1"/>
+      <c r="R92" s="13"/>
+      <c r="S92" s="13"/>
+      <c r="T92" s="13"/>
+      <c r="U92" s="2"/>
+    </row>
+    <row r="93" spans="1:21">
+      <c r="A93" s="21"/>
+      <c r="B93" s="22"/>
+      <c r="C93" s="23"/>
+      <c r="D93" s="25"/>
+      <c r="E93" s="30"/>
+      <c r="F93" s="31"/>
+      <c r="G93" s="35"/>
+      <c r="H93" s="36"/>
+      <c r="I93" s="36"/>
+      <c r="J93" s="37"/>
+      <c r="K93" s="42"/>
+      <c r="L93" s="43"/>
+      <c r="M93" s="46"/>
+      <c r="N93" s="46"/>
+      <c r="O93" s="45"/>
+      <c r="P93" s="44"/>
+      <c r="Q93" s="1"/>
+      <c r="R93" s="13"/>
+      <c r="S93" s="13"/>
+      <c r="T93" s="13"/>
+      <c r="U93" s="2"/>
+    </row>
+    <row r="94" spans="1:21">
+      <c r="A94" s="21"/>
+      <c r="B94" s="22"/>
+      <c r="C94" s="23"/>
+      <c r="D94" s="25"/>
+      <c r="E94" s="30"/>
+      <c r="F94" s="31"/>
+      <c r="G94" s="35"/>
+      <c r="H94" s="36"/>
+      <c r="I94" s="36"/>
+      <c r="J94" s="37"/>
+      <c r="K94" s="42"/>
+      <c r="L94" s="43"/>
+      <c r="M94" s="46"/>
+      <c r="N94" s="46"/>
+      <c r="O94" s="45"/>
+      <c r="P94" s="44"/>
+      <c r="Q94" s="1"/>
+      <c r="R94" s="13"/>
+      <c r="S94" s="13"/>
+      <c r="T94" s="13"/>
+      <c r="U94" s="2"/>
+    </row>
+    <row r="95" spans="1:21">
+      <c r="A95" s="21"/>
+      <c r="B95" s="22"/>
+      <c r="C95" s="23"/>
+      <c r="D95" s="25"/>
+      <c r="E95" s="30"/>
+      <c r="F95" s="31"/>
+      <c r="G95" s="35"/>
+      <c r="H95" s="36"/>
+      <c r="I95" s="36"/>
+      <c r="J95" s="37"/>
+      <c r="K95" s="42"/>
+      <c r="L95" s="43"/>
+      <c r="M95" s="46"/>
+      <c r="N95" s="46"/>
+      <c r="O95" s="45"/>
+      <c r="P95" s="44"/>
+      <c r="Q95" s="1"/>
+      <c r="R95" s="13"/>
+      <c r="S95" s="13"/>
+      <c r="T95" s="13"/>
+      <c r="U95" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="20">
@@ -5265,37 +5687,37 @@
           <x14:formula1>
             <xm:f>DATOS!$D$2:$D$5</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A91</xm:sqref>
+          <xm:sqref>A3:A95</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K91</xm:sqref>
+          <xm:sqref>K3:K95</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$F$2:$F$6</xm:f>
           </x14:formula1>
-          <xm:sqref>L3:L91</xm:sqref>
+          <xm:sqref>L3:L95</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$G$2:$G$3</xm:f>
           </x14:formula1>
-          <xm:sqref>P3:P91</xm:sqref>
+          <xm:sqref>P3:P95</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$C$2:$C$39</xm:f>
           </x14:formula1>
-          <xm:sqref>M3:M91</xm:sqref>
+          <xm:sqref>M3:M95</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$B$2:$B$14</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N91</xm:sqref>
+          <xm:sqref>N3:N95</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>